<commit_message>
Add code to scheduler "main" to read in interventions upon start-up. Remove extra line in .xlsx file for interventions.
</commit_message>
<xml_diff>
--- a/input_files/Interventions.xlsx
+++ b/input_files/Interventions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\CS_4269_Work\Part1\CS4269_Group4_Project\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6434A442-74AA-483D-ADB2-B416D84362FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAFC89D-4BB9-4CCC-BC60-7D4EB0CC1845}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0DBEAA4E-5C28-44EC-BEB5-7DE2FDF83393}"/>
   </bookViews>
@@ -497,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C68CBEA8-BFEF-41B1-9520-7DEA93E453FB}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -611,69 +611,6 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-    </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-    </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-    </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-    </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modify Interventions to increase flexibility.
</commit_message>
<xml_diff>
--- a/input_files/Interventions.xlsx
+++ b/input_files/Interventions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\CS_4269_Work\Part1\CS4269_Group4_Project\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAFC89D-4BB9-4CCC-BC60-7D4EB0CC1845}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDEFA16-0C63-4341-A240-19B58E52A372}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0DBEAA4E-5C28-44EC-BEB5-7DE2FDF83393}"/>
   </bookViews>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Scaling</t>
   </si>
   <si>
-    <t>landArea</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>earthquake</t>
   </si>
   <si>
-    <t>worker_strike</t>
-  </si>
-  <si>
     <t>natural</t>
   </si>
   <si>
@@ -74,19 +68,25 @@
     <t>[population -10%, landArea -5%]</t>
   </si>
   <si>
-    <t>[population -5%]</t>
-  </si>
-  <si>
     <t>[farmLand -25%, landArea -5%]</t>
   </si>
   <si>
-    <t>drought_natural</t>
-  </si>
-  <si>
-    <t>drought_induced</t>
-  </si>
-  <si>
-    <t>farmLand</t>
+    <t>[farmLand 1%]</t>
+  </si>
+  <si>
+    <t>[landArea 0.5%]</t>
+  </si>
+  <si>
+    <t>hurricane</t>
+  </si>
+  <si>
+    <t>[landArea 0.15%]</t>
+  </si>
+  <si>
+    <t>[population -5%, timber -20%, housing -25%]</t>
+  </si>
+  <si>
+    <t>drought</t>
   </si>
 </sst>
 </file>
@@ -499,47 +499,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C68CBEA8-BFEF-41B1-9520-7DEA93E453FB}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="28.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>6</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="D2" s="4">
         <v>1E-4</v>
@@ -548,68 +546,66 @@
         <v>0.05</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3">
         <v>0.02</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="D3" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E3" s="4">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="G3" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3">
         <v>0.03</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="D4" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="G4" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Modify the syntax of scaling and impacts attributes in the Interventions Input File.
</commit_message>
<xml_diff>
--- a/input_files/Interventions.xlsx
+++ b/input_files/Interventions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\CS_4269_Work\Part1\CS4269_Group4_Project\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDEFA16-0C63-4341-A240-19B58E52A372}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F081129-69EE-403A-BD22-8A7DDCB5FA6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0DBEAA4E-5C28-44EC-BEB5-7DE2FDF83393}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Scaling</t>
   </si>
@@ -56,37 +56,34 @@
     <t>earthquake</t>
   </si>
   <si>
-    <t>natural</t>
-  </si>
-  <si>
     <t>deterministic</t>
   </si>
   <si>
     <t>Impacts</t>
   </si>
   <si>
-    <t>[population -10%, landArea -5%]</t>
-  </si>
-  <si>
-    <t>[farmLand -25%, landArea -5%]</t>
-  </si>
-  <si>
-    <t>[farmLand 1%]</t>
-  </si>
-  <si>
-    <t>[landArea 0.5%]</t>
-  </si>
-  <si>
     <t>hurricane</t>
   </si>
   <si>
-    <t>[landArea 0.15%]</t>
-  </si>
-  <si>
-    <t>[population -5%, timber -20%, housing -25%]</t>
-  </si>
-  <si>
     <t>drought</t>
+  </si>
+  <si>
+    <t>{"population" : -.1, "landArea" : -0.05}</t>
+  </si>
+  <si>
+    <t>{"population" : -0.05, "timber" : -0.2, "housing" : -0.25}</t>
+  </si>
+  <si>
+    <t>{"landArea" : 2e-7}</t>
+  </si>
+  <si>
+    <t>{"food" : -0.25, "landArea" : -0.05}</t>
+  </si>
+  <si>
+    <t>{"landArea" : 1.5e-2}</t>
+  </si>
+  <si>
+    <t>{"food" : 1e-5}</t>
   </si>
 </sst>
 </file>
@@ -166,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -181,6 +178,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -497,13 +500,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C68CBEA8-BFEF-41B1-9520-7DEA93E453FB}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="38.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.59765625" customWidth="1"/>
+    <col min="7" max="7" width="50" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -526,7 +532,7 @@
         <v>0</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -534,27 +540,27 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3">
         <v>0</v>
       </c>
       <c r="D2" s="4">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="E2" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="F2" s="2" t="s">
+        <v>0.15</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>7</v>
@@ -568,16 +574,16 @@
       <c r="E3" s="4">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="6" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -591,21 +597,12 @@
       <c r="E4" s="3">
         <v>0.1</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>12</v>
+      <c r="F4" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>